<commit_message>
fix fixture study sheet name
</commit_message>
<xml_diff>
--- a/tests/ARCTokenization.Tests/Fixtures/correct/study_with_source_characteristics_sample.xlsx
+++ b/tests/ARCTokenization.Tests/Fixtures/correct/study_with_source_characteristics_sample.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schne\source\repos\nfdi4plants\ARCTokenization\tests\ARCTokenization.Tests\Fixtures\correct\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{133282B1-8397-4E75-9A5E-2F89F0F98241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C3083AE-B978-48B7-B49F-BA2A20BC70CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="process_sheet_1" sheetId="1" r:id="rId1"/>
-    <sheet name="Study" sheetId="2" r:id="rId2"/>
+    <sheet name="isa_study" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -966,7 +966,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -1045,7 +1045,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A15"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>

</xml_diff>